<commit_message>
Upload Baitap1 lan 2
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\GitHub\Google API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1E8692-BEF4-4662-8D11-C1206CD947BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624BFE2C-B3DC-41E6-AF57-1E9D86BABE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="40">
   <si>
     <t>label</t>
   </si>
@@ -88,28 +88,58 @@
     <t>b'zebra'</t>
   </si>
   <si>
-    <t>b'mt hol'</t>
-  </si>
-  <si>
-    <t>b'bid'</t>
-  </si>
-  <si>
-    <t>b'\xe0\xb4\x86\xe0\xb4\xb0'</t>
-  </si>
-  <si>
-    <t>b'my holi'</t>
-  </si>
-  <si>
-    <t>b'Monkey'</t>
-  </si>
-  <si>
-    <t>b'Question'</t>
-  </si>
-  <si>
-    <t>b'Word'</t>
-  </si>
-  <si>
     <t>% Correct</t>
+  </si>
+  <si>
+    <t>explore</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>joyful</t>
+  </si>
+  <si>
+    <t>monkey</t>
+  </si>
+  <si>
+    <t>pig</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>vehicle</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>yatch</t>
+  </si>
+  <si>
+    <t>zebra</t>
+  </si>
+  <si>
+    <t>mt hol</t>
+  </si>
+  <si>
+    <t>bid</t>
+  </si>
+  <si>
+    <t>\xe0\xb4\x86\xe0\xb4\xb0</t>
+  </si>
+  <si>
+    <t>my holi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monkey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word </t>
   </si>
 </sst>
 </file>
@@ -156,13 +186,19 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -396,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -409,7 +445,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,26 +467,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -768,7 +791,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B1" sqref="B1:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,37 +847,37 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>12</v>
@@ -865,37 +888,37 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>13</v>
@@ -906,37 +929,37 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>14</v>
@@ -947,37 +970,37 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="16" t="s">
         <v>26</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>15</v>
@@ -988,37 +1011,37 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>16</v>
@@ -1029,37 +1052,37 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>17</v>
@@ -1070,37 +1093,37 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>18</v>
@@ -1111,37 +1134,37 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>19</v>
@@ -1152,37 +1175,37 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>20</v>
@@ -1193,28 +1216,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
@@ -1225,7 +1248,7 @@
     </row>
     <row r="12" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C12" s="7">
         <v>1</v>
@@ -1255,16 +1278,16 @@
         <v>0.8</v>
       </c>
       <c r="L12" s="7">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="C2:L11">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>C2&lt;&gt;$B2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>C2=$B2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>